<commit_message>
updated sheets for quick messages
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>TSID</t>
   </si>
@@ -40,10 +40,6 @@
   </si>
   <si>
     <t>Web_SIGNIN</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -926,7 +922,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -960,43 +956,41 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
updated sheets for new & existing messaging and conversation settings
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>TSID</t>
   </si>
@@ -59,7 +59,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Web_URGENT_MESSAGES</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web_FILE_UPLOAD_NEW_USER</t>
+  </si>
+  <si>
+    <t>Web_FILE_UPLOAD_EXISTING_USER</t>
+  </si>
+  <si>
+    <t>Web_CONVERSATIONS</t>
+  </si>
+  <si>
     <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -919,16 +939,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -947,9 +967,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>4</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
@@ -958,9 +976,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>54</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
@@ -969,6 +985,7 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -977,6 +994,9 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="2">
+        <v>63</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
@@ -985,12 +1005,53 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="2">
+        <v>38</v>
+      </c>
       <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>84</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
latest download test sheets
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>TSID</t>
   </si>
@@ -55,27 +55,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Web_URGENT_MESSAGES</t>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_URGENT_MESSAGES</t>
+    <t>Web_FILE_UPLOAD_NEW_USER</t>
+  </si>
+  <si>
+    <t>Web_FILE_UPLOAD_EXISTING_USER</t>
+  </si>
+  <si>
+    <t>Web_CONVERSATIONS</t>
   </si>
   <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_FILE_UPLOAD_NEW_USER</t>
-  </si>
-  <si>
-    <t>Web_FILE_UPLOAD_EXISTING_USER</t>
-  </si>
-  <si>
-    <t>Web_CONVERSATIONS</t>
-  </si>
-  <si>
     <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -942,7 +946,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -978,7 +982,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1009,23 +1013,23 @@
         <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -1034,7 +1038,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>11</v>
@@ -1045,7 +1049,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Aug 8th xlsx commit
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>TSID</t>
   </si>
@@ -75,11 +75,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>N</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -946,7 +950,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -991,7 +995,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1002,7 +1006,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1024,7 +1028,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1033,7 +1037,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1052,10 +1056,11 @@
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
backbone UI change: updated excel sheets as new UI
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-20" windowWidth="23360" windowHeight="12720"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="28000" windowHeight="16020"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>TSID</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Web_QUICK_MESSAGES</t>
-  </si>
-  <si>
-    <t>Web_SIGNOUT</t>
   </si>
   <si>
     <t>Number Of Test Cases</t>
@@ -43,38 +40,61 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Web_SEARCH</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web_URGENT_MESSAGES</t>
+  </si>
+  <si>
+    <t>Web_FILE_UPLOAD_NEW_USER</t>
+  </si>
+  <si>
+    <t>Web_FILE_UPLOAD_EXISTING_USER</t>
+  </si>
+  <si>
+    <t>Web_CONVERSATIONS</t>
+  </si>
+  <si>
+    <t>Web_PATIENT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Web_COMPOSESCREENVALIDATION</t>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_SEARCH</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>Web_GROUPS</t>
+  </si>
+  <si>
+    <t>Web_USERPROFILE</t>
   </si>
   <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_URGENT_MESSAGES</t>
+    <t>Web_CONTACTS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_FILE_UPLOAD_NEW_USER</t>
-  </si>
-  <si>
-    <t>Web_FILE_UPLOAD_EXISTING_USER</t>
-  </si>
-  <si>
-    <t>Web_CONVERSATIONS</t>
-  </si>
-  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Web_SETTINGS</t>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -83,11 +103,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>N</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -95,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -216,6 +236,21 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="25">
@@ -458,7 +493,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -501,6 +536,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -509,7 +546,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1"/>
     <cellStyle name="20% - Accent2" xfId="2"/>
     <cellStyle name="20% - Accent3" xfId="3"/>
@@ -538,11 +575,13 @@
     <cellStyle name="Calculation" xfId="26"/>
     <cellStyle name="Check Cell" xfId="27"/>
     <cellStyle name="Explanatory Text" xfId="28"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="29"/>
     <cellStyle name="Heading 1" xfId="30"/>
     <cellStyle name="Heading 2" xfId="31"/>
     <cellStyle name="Heading 3" xfId="32"/>
     <cellStyle name="Heading 4" xfId="33"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="34"/>
     <cellStyle name="Linked Cell" xfId="35"/>
     <cellStyle name="Neutral" xfId="36"/>
@@ -623,6 +662,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -947,10 +991,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -965,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -973,11 +1017,11 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -986,81 +1030,111 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>63</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
-        <v>38</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>84</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>11</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
change password Eshed feedback: excel sheets
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>TSID</t>
   </si>
@@ -69,18 +69,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Web_CONTACTS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -90,6 +78,10 @@
   </si>
   <si>
     <t>Web_SEARCH</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -222,6 +214,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -979,7 +972,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1006,82 +999,79 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>9</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>12</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1089,31 +1079,34 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
@@ -1123,6 +1116,7 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
excel sheet for workflow test cases 28Sep
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>TSID</t>
   </si>
@@ -65,23 +65,23 @@
     <t>Web_SETTINGS</t>
   </si>
   <si>
+    <t>Web_CONTACTS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web_USERPROFILE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web_SEARCH</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Web_CONTACTS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web_USERPROFILE</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web_SEARCH</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>Web_WORKFLOW</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -214,7 +214,6 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -969,10 +968,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1004,11 +1003,11 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1017,7 +1016,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1025,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1033,7 +1032,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1042,7 +1041,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1050,73 +1049,80 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>11</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Quick message testcases module
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paradigm/dev/CureatrAndroidWorkSpace/InputFiles/Web/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="15940"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="23320" windowHeight="13220"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -94,13 +89,14 @@
   </si>
   <si>
     <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -577,7 +573,7 @@
     <cellStyle name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -973,22 +969,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -999,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1004,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1017,16 +1013,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1034,15 +1030,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1114,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1129,5 +1125,10 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
urgent messages and new message
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27160" windowHeight="13140"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="23080" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -88,11 +88,11 @@
     <t>N</t>
   </si>
   <si>
+    <t>NEW_MESSAGE</t>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEW_MESSAGE</t>
   </si>
   <si>
     <t>Y</t>
@@ -981,7 +981,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1131,13 +1131,14 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>